<commit_message>
Added inverse of to upper level rels
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_Upper_Rels.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_Upper_Rels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgehrk/development/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F07C4C1-0385-3A40-B387-C8C05278BF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D09D55-450D-E64C-8674-F3AD783A9FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="171">
   <si>
     <t>ID</t>
   </si>
@@ -380,9 +380,6 @@
     <t>is behavioural outcome of</t>
   </si>
   <si>
-    <t>inverse 'has behavioural outcome'</t>
-  </si>
-  <si>
     <t>Inverse of has behavioural outcome relation.</t>
   </si>
   <si>
@@ -548,7 +545,7 @@
     <t>material entity</t>
   </si>
   <si>
-    <t>Logical definition</t>
+    <t>Inverse of</t>
   </si>
 </sst>
 </file>
@@ -898,7 +895,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -929,7 +926,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1074,19 +1071,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" t="s">
         <v>162</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>163</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>164</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>165</v>
-      </c>
-      <c r="G9" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1128,22 +1125,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" t="s">
         <v>154</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>155</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>156</v>
-      </c>
-      <c r="E12" t="s">
-        <v>157</v>
       </c>
       <c r="F12" t="s">
         <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1188,16 +1185,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="s">
         <v>117</v>
-      </c>
-      <c r="B15" t="s">
-        <v>118</v>
       </c>
       <c r="D15" t="s">
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F15" t="s">
         <v>29</v>
@@ -1208,22 +1205,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" t="s">
         <v>167</v>
-      </c>
-      <c r="B16" t="s">
-        <v>168</v>
       </c>
       <c r="D16" t="s">
         <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F16" t="s">
         <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1274,24 +1271,24 @@
         <v>114</v>
       </c>
       <c r="E19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H19" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
         <v>139</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>140</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>141</v>
-      </c>
-      <c r="E20" t="s">
-        <v>142</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
@@ -1316,41 +1313,41 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" t="s">
         <v>146</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>147</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>148</v>
-      </c>
-      <c r="E22" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" t="s">
         <v>150</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>151</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>152</v>
-      </c>
-      <c r="E23" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" t="s">
         <v>132</v>
       </c>
-      <c r="B24" t="s">
+      <c r="E24" t="s">
         <v>133</v>
-      </c>
-      <c r="E24" t="s">
-        <v>134</v>
       </c>
       <c r="F24" t="s">
         <v>29</v>
@@ -1389,30 +1386,30 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" t="s">
         <v>120</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>121</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>122</v>
-      </c>
-      <c r="E27" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
         <v>128</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>129</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>130</v>
-      </c>
-      <c r="E28" t="s">
-        <v>131</v>
       </c>
       <c r="F28" t="s">
         <v>54</v>
@@ -1465,16 +1462,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s">
         <v>143</v>
-      </c>
-      <c r="B32" t="s">
-        <v>144</v>
       </c>
       <c r="C32" t="s">
         <v>51</v>
       </c>
       <c r="E32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1493,16 +1490,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" t="s">
         <v>124</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>125</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>126</v>
-      </c>
-      <c r="E34" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1527,16 +1524,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" t="s">
         <v>159</v>
-      </c>
-      <c r="B36" t="s">
-        <v>160</v>
       </c>
       <c r="D36" t="s">
         <v>27</v>
       </c>
       <c r="E36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F36" t="s">
         <v>29</v>
@@ -1581,16 +1578,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" t="s">
         <v>135</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>136</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>137</v>
-      </c>
-      <c r="E39" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>